<commit_message>
added back editDocumentPage tests and they all pass
</commit_message>
<xml_diff>
--- a/backend/data.xlsx
+++ b/backend/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="18">
   <si>
     <t>Invoice ID</t>
   </si>
@@ -441,7 +441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="6" width="15" customWidth="1"/>
@@ -720,6 +720,20 @@
         <v>16</v>
       </c>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>